<commit_message>
new version - turn on dilute bit, also move to subdirectory, which arduino software seems to prefer
</commit_message>
<xml_diff>
--- a/DSAMLookupDefinitions.xlsx
+++ b/DSAMLookupDefinitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\arduino\pohlman\dsamcontroller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\arduino\pohlman\DSAM_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="LookupTable" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">LookupTable!$A$1:$BA$30</definedName>
@@ -27,8 +28,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Marinna Martini</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Marinna Martini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+these pins are set discretely during the setup function call</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Purge SW</t>
   </si>
@@ -61,9 +96,6 @@
   </si>
   <si>
     <t>Dilute</t>
-  </si>
-  <si>
-    <t>LEDWord</t>
   </si>
   <si>
     <t>K6 - 40 - PG1</t>
@@ -186,9 +218,6 @@
     <t>this command is executed as dilute B for 2 sec, then analyze</t>
   </si>
   <si>
-    <t>Instantiate</t>
-  </si>
-  <si>
     <t>Pin</t>
   </si>
   <si>
@@ -201,17 +230,26 @@
     <t>pinsToSet</t>
   </si>
   <si>
-    <t>buttonWord</t>
+    <t>DSAM Logic table</t>
   </si>
   <si>
-    <t>DSAM Logic table</t>
+    <t>last col</t>
+  </si>
+  <si>
+    <t>LEDWord, 0 = LED lit</t>
+  </si>
+  <si>
+    <t>buttonWord, 0 = button depressed</t>
+  </si>
+  <si>
+    <t>Initiate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +263,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,7 +323,487 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="132">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -728,14 +1259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC13" sqref="AC13"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,10 +1284,10 @@
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -775,7 +1306,7 @@
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U1" s="7"/>
       <c r="V1" s="7"/>
@@ -794,7 +1325,7 @@
       <c r="AI1" s="7"/>
       <c r="AJ1" s="7"/>
       <c r="AK1" s="7" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="AL1" s="7"/>
       <c r="AM1" s="7"/>
@@ -816,7 +1347,7 @@
     <row r="2" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <f ca="1">NOW()</f>
-        <v>42726.369925462961</v>
+        <v>42752.556931481478</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
@@ -828,12 +1359,12 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -866,12 +1397,12 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
       <c r="AS2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AT2" s="7"/>
       <c r="AU2" s="7"/>
       <c r="AV2" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AW2" s="7"/>
       <c r="AX2" s="7"/>
@@ -881,7 +1412,7 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -988,39 +1519,39 @@
         <v>30</v>
       </c>
       <c r="AZ3" s="5">
+        <v>53</v>
+      </c>
+      <c r="BA3" s="5">
         <v>52</v>
       </c>
-      <c r="BA3" s="5">
-        <v>53</v>
-      </c>
     </row>
-    <row r="4" spans="1:53" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:53" ht="62" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>0</v>
@@ -1044,94 +1575,94 @@
         <v>7</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="T4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="AV4" s="1" t="s">
         <v>3</v>
@@ -1146,15 +1677,15 @@
         <v>7</v>
       </c>
       <c r="AZ4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="BA4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <f>D5*2^15+E5*2^14+F5*2^13+G5*2^12+H5*2^11+I5*2^10+J5*2^9+K5*2^8+L5*2^7+M5*2^6+N5*2^5+O5*2^4+P5*2^3+Q5*2^2+R5*2+S5</f>
@@ -1262,55 +1793,55 @@
       </c>
       <c r="AK5">
         <f>AL5*2^15+AM5*2^14+AN5*2^13+AO5*2^12+AP5*2^11+AQ5*2^10+AR5*2^9+AS5*2^8+AT5*2^7+AU5*2^6+AV5*2^5+AW5*2^4+AX5*2^3+AY5*2^2+AZ5*2+BA5</f>
-        <v>0</v>
+        <v>65535</v>
       </c>
       <c r="AL5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.35">
@@ -1476,7 +2007,7 @@
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C30" si="0">D7*2^15+E7*2^14+F7*2^13+G7*2^12+H7*2^11+I7*2^10+J7*2^9+K7*2^8+L7*2^7+M7*2^6+N7*2^5+O7*2^4+P7*2^3+Q7*2^2+R7*2+S7</f>
@@ -1637,7 +2168,7 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1798,7 +2329,7 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1959,7 +2490,7 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -2120,7 +2651,7 @@
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -2281,7 +2812,7 @@
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -2442,7 +2973,7 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -2603,7 +3134,7 @@
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -2764,7 +3295,7 @@
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -2925,7 +3456,7 @@
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -3086,7 +3617,7 @@
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -3251,7 +3782,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>65533</v>
+        <v>65534</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -3295,11 +3826,11 @@
       <c r="Q18" s="4">
         <v>1</v>
       </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18" s="4">
-        <v>1</v>
+      <c r="R18" s="4">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
       </c>
       <c r="T18">
         <f t="shared" si="1"/>
@@ -3355,7 +3886,7 @@
       </c>
       <c r="AK18">
         <f t="shared" si="2"/>
-        <v>65533</v>
+        <v>65534</v>
       </c>
       <c r="AL18" s="4">
         <v>1</v>
@@ -3400,19 +3931,19 @@
         <v>1</v>
       </c>
       <c r="AZ18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19" si="3">D19*2^15+E19*2^14+F19*2^13+G19*2^12+H19*2^11+I19*2^10+J19*2^9+K19*2^8+L19*2^7+M19*2^6+N19*2^5+O19*2^4+P19*2^3+Q19*2^2+R19*2+S19</f>
-        <v>65438</v>
+        <v>65437</v>
       </c>
       <c r="D19">
         <f>IF(AND(D20:D21),1,0)</f>
@@ -3472,91 +4003,89 @@
       </c>
       <c r="R19">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="S19" si="5">IF(AND(S20:S21),1,0)</f>
+        <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AK19">
         <f t="shared" si="2"/>
-        <v>65438</v>
+        <v>65437</v>
       </c>
       <c r="AL19">
         <f>IF(AND(AL20:AL21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AM19">
-        <f t="shared" ref="AM19" si="5">IF(AND(AM20:AM21),1,0)</f>
+        <f t="shared" ref="AM19" si="6">IF(AND(AM20:AM21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AN19">
-        <f t="shared" ref="AN19" si="6">IF(AND(AN20:AN21),1,0)</f>
+        <f t="shared" ref="AN19" si="7">IF(AND(AN20:AN21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AO19">
-        <f t="shared" ref="AO19" si="7">IF(AND(AO20:AO21),1,0)</f>
+        <f t="shared" ref="AO19" si="8">IF(AND(AO20:AO21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AP19">
-        <f t="shared" ref="AP19" si="8">IF(AND(AP20:AP21),1,0)</f>
+        <f t="shared" ref="AP19" si="9">IF(AND(AP20:AP21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AQ19">
-        <f t="shared" ref="AQ19" si="9">IF(AND(AQ20:AQ21),1,0)</f>
+        <f t="shared" ref="AQ19" si="10">IF(AND(AQ20:AQ21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AR19">
-        <f t="shared" ref="AR19" si="10">IF(AND(AR20:AR21),1,0)</f>
+        <f t="shared" ref="AR19" si="11">IF(AND(AR20:AR21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AS19">
-        <f t="shared" ref="AS19" si="11">IF(AND(AS20:AS21),1,0)</f>
+        <f t="shared" ref="AS19" si="12">IF(AND(AS20:AS21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AT19">
-        <f t="shared" ref="AT19" si="12">IF(AND(AT20:AT21),1,0)</f>
+        <f t="shared" ref="AT19" si="13">IF(AND(AT20:AT21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AU19">
-        <f t="shared" ref="AU19" si="13">IF(AND(AU20:AU21),1,0)</f>
+        <f t="shared" ref="AU19" si="14">IF(AND(AU20:AU21),1,0)</f>
         <v>0</v>
       </c>
       <c r="AV19">
-        <f t="shared" ref="AV19" si="14">IF(AND(AV20:AV21),1,0)</f>
+        <f t="shared" ref="AV19" si="15">IF(AND(AV20:AV21),1,0)</f>
         <v>0</v>
       </c>
       <c r="AW19">
-        <f t="shared" ref="AW19" si="15">IF(AND(AW20:AW21),1,0)</f>
+        <f t="shared" ref="AW19" si="16">IF(AND(AW20:AW21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AX19">
-        <f t="shared" ref="AX19" si="16">IF(AND(AX20:AX21),1,0)</f>
+        <f t="shared" ref="AX19" si="17">IF(AND(AX20:AX21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AY19">
-        <f t="shared" ref="AY19" si="17">IF(AND(AY20:AY21),1,0)</f>
+        <f t="shared" ref="AY19:BA19" si="18">IF(AND(AY20:AY21),1,0)</f>
         <v>1</v>
       </c>
       <c r="AZ19">
-        <f t="shared" ref="AZ19" si="18">IF(AND(AZ20:AZ21),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA19">
-        <f t="shared" ref="BA19" si="19">IF(AND(BA20:BA21),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>65438</v>
+        <v>65437</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3600,11 +4129,11 @@
       <c r="Q20" s="4">
         <v>1</v>
       </c>
-      <c r="R20" s="4">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>1</v>
       </c>
       <c r="T20">
         <f t="shared" si="1"/>
@@ -3660,7 +4189,7 @@
       </c>
       <c r="AK20">
         <f t="shared" si="2"/>
-        <v>65438</v>
+        <v>65437</v>
       </c>
       <c r="AL20" s="4">
         <v>1</v>
@@ -3705,15 +4234,15 @@
         <v>1</v>
       </c>
       <c r="AZ20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -3874,155 +4403,153 @@
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>65454</v>
+        <v>65453</v>
       </c>
       <c r="D22">
         <f>IF(AND(D23:D24),1,0)</f>
         <v>1</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22" si="20">IF(AND(E23:E24),1,0)</f>
+        <f t="shared" ref="E22" si="19">IF(AND(E23:E24),1,0)</f>
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22" si="21">IF(AND(F23:F24),1,0)</f>
+        <f t="shared" ref="F22" si="20">IF(AND(F23:F24),1,0)</f>
         <v>1</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22" si="22">IF(AND(G23:G24),1,0)</f>
+        <f t="shared" ref="G22" si="21">IF(AND(G23:G24),1,0)</f>
         <v>1</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22" si="23">IF(AND(H23:H24),1,0)</f>
+        <f t="shared" ref="H22" si="22">IF(AND(H23:H24),1,0)</f>
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22" si="24">IF(AND(I23:I24),1,0)</f>
+        <f t="shared" ref="I22" si="23">IF(AND(I23:I24),1,0)</f>
         <v>1</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22" si="25">IF(AND(J23:J24),1,0)</f>
+        <f t="shared" ref="J22" si="24">IF(AND(J23:J24),1,0)</f>
         <v>1</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22" si="26">IF(AND(K23:K24),1,0)</f>
+        <f t="shared" ref="K22" si="25">IF(AND(K23:K24),1,0)</f>
         <v>1</v>
       </c>
       <c r="L22">
-        <f t="shared" ref="L22" si="27">IF(AND(L23:L24),1,0)</f>
+        <f t="shared" ref="L22" si="26">IF(AND(L23:L24),1,0)</f>
         <v>1</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22" si="28">IF(AND(M23:M24),1,0)</f>
+        <f t="shared" ref="M22" si="27">IF(AND(M23:M24),1,0)</f>
         <v>0</v>
       </c>
       <c r="N22">
-        <f t="shared" ref="N22" si="29">IF(AND(N23:N24),1,0)</f>
+        <f t="shared" ref="N22" si="28">IF(AND(N23:N24),1,0)</f>
         <v>1</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="O22" si="30">IF(AND(O23:O24),1,0)</f>
+        <f t="shared" ref="O22" si="29">IF(AND(O23:O24),1,0)</f>
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" ref="P22" si="31">IF(AND(P23:P24),1,0)</f>
+        <f t="shared" ref="P22" si="30">IF(AND(P23:P24),1,0)</f>
         <v>1</v>
       </c>
       <c r="Q22">
-        <f t="shared" ref="Q22" si="32">IF(AND(Q23:Q24),1,0)</f>
+        <f t="shared" ref="Q22:R22" si="31">IF(AND(Q23:Q24),1,0)</f>
         <v>1</v>
       </c>
       <c r="R22">
-        <f t="shared" ref="R22" si="33">IF(AND(R23:R24),1,0)</f>
-        <v>1</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22" si="34">IF(AND(S23:S24),1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="R22:S22" si="32">IF(AND(S23:S24),1,0)</f>
+        <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AK22">
-        <f t="shared" ref="AK22" si="35">AL22*2^15+AM22*2^14+AN22*2^13+AO22*2^12+AP22*2^11+AQ22*2^10+AR22*2^9+AS22*2^8+AT22*2^7+AU22*2^6+AV22*2^5+AW22*2^4+AX22*2^3+AY22*2^2+AZ22*2+BA22</f>
-        <v>65454</v>
+        <f t="shared" ref="AK22" si="33">AL22*2^15+AM22*2^14+AN22*2^13+AO22*2^12+AP22*2^11+AQ22*2^10+AR22*2^9+AS22*2^8+AT22*2^7+AU22*2^6+AV22*2^5+AW22*2^4+AX22*2^3+AY22*2^2+AZ22*2+BA22</f>
+        <v>65453</v>
       </c>
       <c r="AL22">
         <f>IF(AND(AL23:AL24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AM22">
-        <f t="shared" ref="AM22" si="36">IF(AND(AM23:AM24),1,0)</f>
+        <f t="shared" ref="AM22" si="34">IF(AND(AM23:AM24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AN22">
-        <f t="shared" ref="AN22" si="37">IF(AND(AN23:AN24),1,0)</f>
+        <f t="shared" ref="AN22" si="35">IF(AND(AN23:AN24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AO22">
-        <f t="shared" ref="AO22" si="38">IF(AND(AO23:AO24),1,0)</f>
+        <f t="shared" ref="AO22" si="36">IF(AND(AO23:AO24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AP22">
-        <f t="shared" ref="AP22" si="39">IF(AND(AP23:AP24),1,0)</f>
+        <f t="shared" ref="AP22" si="37">IF(AND(AP23:AP24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AQ22">
-        <f t="shared" ref="AQ22" si="40">IF(AND(AQ23:AQ24),1,0)</f>
+        <f t="shared" ref="AQ22" si="38">IF(AND(AQ23:AQ24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AR22">
-        <f t="shared" ref="AR22" si="41">IF(AND(AR23:AR24),1,0)</f>
+        <f t="shared" ref="AR22" si="39">IF(AND(AR23:AR24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AS22">
-        <f t="shared" ref="AS22" si="42">IF(AND(AS23:AS24),1,0)</f>
+        <f t="shared" ref="AS22" si="40">IF(AND(AS23:AS24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AT22">
-        <f t="shared" ref="AT22" si="43">IF(AND(AT23:AT24),1,0)</f>
+        <f t="shared" ref="AT22" si="41">IF(AND(AT23:AT24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AU22">
-        <f t="shared" ref="AU22" si="44">IF(AND(AU23:AU24),1,0)</f>
+        <f t="shared" ref="AU22" si="42">IF(AND(AU23:AU24),1,0)</f>
         <v>0</v>
       </c>
       <c r="AV22">
-        <f t="shared" ref="AV22" si="45">IF(AND(AV23:AV24),1,0)</f>
+        <f t="shared" ref="AV22" si="43">IF(AND(AV23:AV24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AW22">
-        <f t="shared" ref="AW22" si="46">IF(AND(AW23:AW24),1,0)</f>
+        <f t="shared" ref="AW22" si="44">IF(AND(AW23:AW24),1,0)</f>
         <v>0</v>
       </c>
       <c r="AX22">
-        <f t="shared" ref="AX22" si="47">IF(AND(AX23:AX24),1,0)</f>
+        <f t="shared" ref="AX22" si="45">IF(AND(AX23:AX24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AY22">
-        <f t="shared" ref="AY22" si="48">IF(AND(AY23:AY24),1,0)</f>
+        <f t="shared" ref="AY22:BA22" si="46">IF(AND(AY23:AY24),1,0)</f>
         <v>1</v>
       </c>
       <c r="AZ22">
-        <f t="shared" ref="AZ22" si="49">IF(AND(AZ23:AZ24),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA22">
-        <f t="shared" ref="BA22" si="50">IF(AND(BA23:BA24),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>65454</v>
+        <v>65453</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -4066,11 +4593,11 @@
       <c r="Q23" s="4">
         <v>1</v>
       </c>
-      <c r="R23" s="4">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" s="4">
+        <v>1</v>
       </c>
       <c r="T23">
         <f t="shared" si="1"/>
@@ -4126,7 +4653,7 @@
       </c>
       <c r="AK23">
         <f t="shared" si="2"/>
-        <v>65454</v>
+        <v>65453</v>
       </c>
       <c r="AL23" s="4">
         <v>1</v>
@@ -4171,15 +4698,15 @@
         <v>1</v>
       </c>
       <c r="AZ23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
@@ -4340,155 +4867,153 @@
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25" si="51">D25*2^15+E25*2^14+F25*2^13+G25*2^12+H25*2^11+I25*2^10+J25*2^9+K25*2^8+L25*2^7+M25*2^6+N25*2^5+O25*2^4+P25*2^3+Q25*2^2+R25*2+S25</f>
-        <v>65462</v>
+        <f t="shared" ref="C25" si="47">D25*2^15+E25*2^14+F25*2^13+G25*2^12+H25*2^11+I25*2^10+J25*2^9+K25*2^8+L25*2^7+M25*2^6+N25*2^5+O25*2^4+P25*2^3+Q25*2^2+R25*2+S25</f>
+        <v>65461</v>
       </c>
       <c r="D25">
         <f>IF(AND(D26:D27),1,0)</f>
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25" si="52">IF(AND(E26:E27),1,0)</f>
+        <f t="shared" ref="E25" si="48">IF(AND(E26:E27),1,0)</f>
         <v>1</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25" si="53">IF(AND(F26:F27),1,0)</f>
+        <f t="shared" ref="F25" si="49">IF(AND(F26:F27),1,0)</f>
         <v>1</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25" si="54">IF(AND(G26:G27),1,0)</f>
+        <f t="shared" ref="G25" si="50">IF(AND(G26:G27),1,0)</f>
         <v>1</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25" si="55">IF(AND(H26:H27),1,0)</f>
+        <f t="shared" ref="H25" si="51">IF(AND(H26:H27),1,0)</f>
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25" si="56">IF(AND(I26:I27),1,0)</f>
+        <f t="shared" ref="I25" si="52">IF(AND(I26:I27),1,0)</f>
         <v>1</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25" si="57">IF(AND(J26:J27),1,0)</f>
+        <f t="shared" ref="J25" si="53">IF(AND(J26:J27),1,0)</f>
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25" si="58">IF(AND(K26:K27),1,0)</f>
+        <f t="shared" ref="K25" si="54">IF(AND(K26:K27),1,0)</f>
         <v>1</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25" si="59">IF(AND(L26:L27),1,0)</f>
+        <f t="shared" ref="L25" si="55">IF(AND(L26:L27),1,0)</f>
         <v>1</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25" si="60">IF(AND(M26:M27),1,0)</f>
+        <f t="shared" ref="M25" si="56">IF(AND(M26:M27),1,0)</f>
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25" si="61">IF(AND(N26:N27),1,0)</f>
+        <f t="shared" ref="N25" si="57">IF(AND(N26:N27),1,0)</f>
         <v>1</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25" si="62">IF(AND(O26:O27),1,0)</f>
+        <f t="shared" ref="O25" si="58">IF(AND(O26:O27),1,0)</f>
         <v>1</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25" si="63">IF(AND(P26:P27),1,0)</f>
+        <f t="shared" ref="P25" si="59">IF(AND(P26:P27),1,0)</f>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25" si="64">IF(AND(Q26:Q27),1,0)</f>
+        <f t="shared" ref="Q25:R25" si="60">IF(AND(Q26:Q27),1,0)</f>
         <v>1</v>
       </c>
       <c r="R25">
-        <f t="shared" ref="R25" si="65">IF(AND(R26:R27),1,0)</f>
-        <v>1</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="S25">
-        <f t="shared" ref="S25" si="66">IF(AND(S26:S27),1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="R25:S25" si="61">IF(AND(S26:S27),1,0)</f>
+        <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AK25">
         <f t="shared" si="2"/>
-        <v>65462</v>
+        <v>65461</v>
       </c>
       <c r="AL25">
         <f>IF(AND(AL26:AL27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AM25">
-        <f t="shared" ref="AM25" si="67">IF(AND(AM26:AM27),1,0)</f>
+        <f t="shared" ref="AM25" si="62">IF(AND(AM26:AM27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AN25">
-        <f t="shared" ref="AN25" si="68">IF(AND(AN26:AN27),1,0)</f>
+        <f t="shared" ref="AN25" si="63">IF(AND(AN26:AN27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AO25">
-        <f t="shared" ref="AO25" si="69">IF(AND(AO26:AO27),1,0)</f>
+        <f t="shared" ref="AO25" si="64">IF(AND(AO26:AO27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AP25">
-        <f t="shared" ref="AP25" si="70">IF(AND(AP26:AP27),1,0)</f>
+        <f t="shared" ref="AP25" si="65">IF(AND(AP26:AP27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AQ25">
-        <f t="shared" ref="AQ25" si="71">IF(AND(AQ26:AQ27),1,0)</f>
+        <f t="shared" ref="AQ25" si="66">IF(AND(AQ26:AQ27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AR25">
-        <f t="shared" ref="AR25" si="72">IF(AND(AR26:AR27),1,0)</f>
+        <f t="shared" ref="AR25" si="67">IF(AND(AR26:AR27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AS25">
-        <f t="shared" ref="AS25" si="73">IF(AND(AS26:AS27),1,0)</f>
+        <f t="shared" ref="AS25" si="68">IF(AND(AS26:AS27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AT25">
-        <f t="shared" ref="AT25" si="74">IF(AND(AT26:AT27),1,0)</f>
+        <f t="shared" ref="AT25" si="69">IF(AND(AT26:AT27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AU25">
-        <f t="shared" ref="AU25" si="75">IF(AND(AU26:AU27),1,0)</f>
+        <f t="shared" ref="AU25" si="70">IF(AND(AU26:AU27),1,0)</f>
         <v>0</v>
       </c>
       <c r="AV25">
-        <f t="shared" ref="AV25" si="76">IF(AND(AV26:AV27),1,0)</f>
+        <f t="shared" ref="AV25" si="71">IF(AND(AV26:AV27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AW25">
-        <f t="shared" ref="AW25" si="77">IF(AND(AW26:AW27),1,0)</f>
+        <f t="shared" ref="AW25" si="72">IF(AND(AW26:AW27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AX25">
-        <f t="shared" ref="AX25" si="78">IF(AND(AX26:AX27),1,0)</f>
+        <f t="shared" ref="AX25" si="73">IF(AND(AX26:AX27),1,0)</f>
         <v>0</v>
       </c>
       <c r="AY25">
-        <f t="shared" ref="AY25" si="79">IF(AND(AY26:AY27),1,0)</f>
+        <f t="shared" ref="AY25:BA25" si="74">IF(AND(AY26:AY27),1,0)</f>
         <v>1</v>
       </c>
       <c r="AZ25">
-        <f t="shared" ref="AZ25" si="80">IF(AND(AZ26:AZ27),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA25">
-        <f t="shared" ref="BA25" si="81">IF(AND(BA26:BA27),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>65462</v>
+        <v>65461</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -4532,11 +5057,11 @@
       <c r="Q26" s="4">
         <v>1</v>
       </c>
-      <c r="R26" s="4">
-        <v>1</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26" s="4">
+        <v>1</v>
       </c>
       <c r="T26">
         <f t="shared" si="1"/>
@@ -4592,7 +5117,7 @@
       </c>
       <c r="AK26">
         <f t="shared" si="2"/>
-        <v>65462</v>
+        <v>65461</v>
       </c>
       <c r="AL26" s="4">
         <v>1</v>
@@ -4637,15 +5162,15 @@
         <v>1</v>
       </c>
       <c r="AZ26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
@@ -4806,155 +5331,153 @@
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28" si="82">D28*2^15+E28*2^14+F28*2^13+G28*2^12+H28*2^11+I28*2^10+J28*2^9+K28*2^8+L28*2^7+M28*2^6+N28*2^5+O28*2^4+P28*2^3+Q28*2^2+R28*2+S28</f>
-        <v>65466</v>
+        <f t="shared" ref="C28" si="75">D28*2^15+E28*2^14+F28*2^13+G28*2^12+H28*2^11+I28*2^10+J28*2^9+K28*2^8+L28*2^7+M28*2^6+N28*2^5+O28*2^4+P28*2^3+Q28*2^2+R28*2+S28</f>
+        <v>65465</v>
       </c>
       <c r="D28">
         <f>IF(AND(D29:D30),1,0)</f>
         <v>1</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28" si="83">IF(AND(E29:E30),1,0)</f>
+        <f t="shared" ref="E28" si="76">IF(AND(E29:E30),1,0)</f>
         <v>1</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28" si="84">IF(AND(F29:F30),1,0)</f>
+        <f t="shared" ref="F28" si="77">IF(AND(F29:F30),1,0)</f>
         <v>1</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28" si="85">IF(AND(G29:G30),1,0)</f>
+        <f t="shared" ref="G28" si="78">IF(AND(G29:G30),1,0)</f>
         <v>1</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28" si="86">IF(AND(H29:H30),1,0)</f>
+        <f t="shared" ref="H28" si="79">IF(AND(H29:H30),1,0)</f>
         <v>1</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28" si="87">IF(AND(I29:I30),1,0)</f>
+        <f t="shared" ref="I28" si="80">IF(AND(I29:I30),1,0)</f>
         <v>1</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28" si="88">IF(AND(J29:J30),1,0)</f>
+        <f t="shared" ref="J28" si="81">IF(AND(J29:J30),1,0)</f>
         <v>1</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28" si="89">IF(AND(K29:K30),1,0)</f>
+        <f t="shared" ref="K28" si="82">IF(AND(K29:K30),1,0)</f>
         <v>1</v>
       </c>
       <c r="L28">
-        <f t="shared" ref="L28" si="90">IF(AND(L29:L30),1,0)</f>
+        <f t="shared" ref="L28" si="83">IF(AND(L29:L30),1,0)</f>
         <v>1</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28" si="91">IF(AND(M29:M30),1,0)</f>
+        <f t="shared" ref="M28" si="84">IF(AND(M29:M30),1,0)</f>
         <v>0</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28" si="92">IF(AND(N29:N30),1,0)</f>
+        <f t="shared" ref="N28" si="85">IF(AND(N29:N30),1,0)</f>
         <v>1</v>
       </c>
       <c r="O28">
-        <f t="shared" ref="O28" si="93">IF(AND(O29:O30),1,0)</f>
+        <f t="shared" ref="O28" si="86">IF(AND(O29:O30),1,0)</f>
         <v>1</v>
       </c>
       <c r="P28">
-        <f t="shared" ref="P28" si="94">IF(AND(P29:P30),1,0)</f>
+        <f t="shared" ref="P28" si="87">IF(AND(P29:P30),1,0)</f>
         <v>1</v>
       </c>
       <c r="Q28">
-        <f t="shared" ref="Q28" si="95">IF(AND(Q29:Q30),1,0)</f>
+        <f t="shared" ref="Q28:R28" si="88">IF(AND(Q29:Q30),1,0)</f>
         <v>0</v>
       </c>
       <c r="R28">
-        <f t="shared" ref="R28" si="96">IF(AND(R29:R30),1,0)</f>
-        <v>1</v>
+        <f t="shared" si="88"/>
+        <v>0</v>
       </c>
       <c r="S28">
-        <f t="shared" ref="S28" si="97">IF(AND(S29:S30),1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="R28:S28" si="89">IF(AND(S29:S30),1,0)</f>
+        <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AK28">
         <f t="shared" si="2"/>
-        <v>65466</v>
+        <v>65465</v>
       </c>
       <c r="AL28">
         <f>IF(AND(AL29:AL30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AM28">
-        <f t="shared" ref="AM28" si="98">IF(AND(AM29:AM30),1,0)</f>
+        <f t="shared" ref="AM28" si="90">IF(AND(AM29:AM30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AN28">
-        <f t="shared" ref="AN28" si="99">IF(AND(AN29:AN30),1,0)</f>
+        <f t="shared" ref="AN28" si="91">IF(AND(AN29:AN30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AO28">
-        <f t="shared" ref="AO28" si="100">IF(AND(AO29:AO30),1,0)</f>
+        <f t="shared" ref="AO28" si="92">IF(AND(AO29:AO30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AP28">
-        <f t="shared" ref="AP28" si="101">IF(AND(AP29:AP30),1,0)</f>
+        <f t="shared" ref="AP28" si="93">IF(AND(AP29:AP30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AQ28">
-        <f t="shared" ref="AQ28" si="102">IF(AND(AQ29:AQ30),1,0)</f>
+        <f t="shared" ref="AQ28" si="94">IF(AND(AQ29:AQ30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AR28">
-        <f t="shared" ref="AR28" si="103">IF(AND(AR29:AR30),1,0)</f>
+        <f t="shared" ref="AR28" si="95">IF(AND(AR29:AR30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AS28">
-        <f t="shared" ref="AS28" si="104">IF(AND(AS29:AS30),1,0)</f>
+        <f t="shared" ref="AS28" si="96">IF(AND(AS29:AS30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AT28">
-        <f t="shared" ref="AT28" si="105">IF(AND(AT29:AT30),1,0)</f>
+        <f t="shared" ref="AT28" si="97">IF(AND(AT29:AT30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AU28">
-        <f t="shared" ref="AU28" si="106">IF(AND(AU29:AU30),1,0)</f>
+        <f t="shared" ref="AU28" si="98">IF(AND(AU29:AU30),1,0)</f>
         <v>0</v>
       </c>
       <c r="AV28">
-        <f t="shared" ref="AV28" si="107">IF(AND(AV29:AV30),1,0)</f>
+        <f t="shared" ref="AV28" si="99">IF(AND(AV29:AV30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AW28">
-        <f t="shared" ref="AW28" si="108">IF(AND(AW29:AW30),1,0)</f>
+        <f t="shared" ref="AW28" si="100">IF(AND(AW29:AW30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AX28">
-        <f t="shared" ref="AX28" si="109">IF(AND(AX29:AX30),1,0)</f>
+        <f t="shared" ref="AX28" si="101">IF(AND(AX29:AX30),1,0)</f>
         <v>1</v>
       </c>
       <c r="AY28">
-        <f t="shared" ref="AY28" si="110">IF(AND(AY29:AY30),1,0)</f>
+        <f t="shared" ref="AY28:BA28" si="102">IF(AND(AY29:AY30),1,0)</f>
         <v>0</v>
       </c>
       <c r="AZ28">
-        <f t="shared" ref="AZ28" si="111">IF(AND(AZ29:AZ30),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA28">
-        <f t="shared" ref="BA28" si="112">IF(AND(BA29:BA30),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>65466</v>
+        <v>65465</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -4998,11 +5521,11 @@
       <c r="Q29">
         <v>0</v>
       </c>
-      <c r="R29" s="4">
-        <v>1</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29" s="4">
+        <v>1</v>
       </c>
       <c r="T29">
         <f t="shared" si="1"/>
@@ -5058,7 +5581,7 @@
       </c>
       <c r="AK29">
         <f t="shared" si="2"/>
-        <v>65466</v>
+        <v>65465</v>
       </c>
       <c r="AL29" s="4">
         <v>1</v>
@@ -5103,15 +5626,15 @@
         <v>0</v>
       </c>
       <c r="AZ29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
@@ -5281,147 +5804,243 @@
     <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="AV2:AY2"/>
   </mergeCells>
-  <conditionalFormatting sqref="K6:S18 K20:S21 K23:S24 K26:S27 K29:S30">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+  <conditionalFormatting sqref="K6:Q18 K20:Q21 K23:Q24 K26:Q27 K29:Q30">
+    <cfRule type="cellIs" dxfId="131" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6:AJ18 Y20:AJ21 Y23:AJ24 Y26:AJ27 Y29:AJ30">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="57" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS6:BA18 AS20:BA21 AS23:BA24 AS26:BA27 AS29:BA30">
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL19:BA19">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19:S19">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+  <conditionalFormatting sqref="D19:Q19">
+    <cfRule type="cellIs" dxfId="123" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19:AJ19">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL22:BA22">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28:BA28">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:S22">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+  <conditionalFormatting sqref="D22:Q22">
+    <cfRule type="cellIs" dxfId="115" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22:AJ22">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL25:BA25">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:S25">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+  <conditionalFormatting sqref="D25:Q25">
+    <cfRule type="cellIs" dxfId="109" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U25:AJ25">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:S28">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="D28:Q28">
+    <cfRule type="cellIs" dxfId="105" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28:AJ28">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:S5">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="K5:Q5">
+    <cfRule type="cellIs" dxfId="101" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y5:AJ5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS5:BA5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S6:S18 S20:S21 S23:S24 S26:S27 S29:S30">
+    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S19">
+    <cfRule type="cellIs" dxfId="67" priority="21" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="22" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S22">
+    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S25">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="18" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S28">
+    <cfRule type="cellIs" dxfId="55" priority="15" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="16" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5">
+    <cfRule type="cellIs" dxfId="51" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R6:R18 R20:R21 R23:R24 R26:R27 R29:R30">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19">
+    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R22">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R28">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5430,5 +6049,208 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="36" max="26" man="1"/>
   </colBreaks>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F4:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <f t="shared" ref="F19" si="0">IF(AND(F20:F21),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <f t="shared" ref="F22" si="1">IF(AND(F23:F24),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <f t="shared" ref="F25" si="2">IF(AND(F26:F27),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <f t="shared" ref="F28" si="3">IF(AND(F29:F30),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F6:F18 F20:F21 F23:F24 F26:F27 F29:F30">
+    <cfRule type="cellIs" dxfId="95" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="cellIs" dxfId="91" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="83" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>